<commit_message>
[전인호] tube.xlsx jakeR, doncina01, doncina02 튜브 추가
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/tube.xlsx
+++ b/DesignDocs/VariableData/tube.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613FE9C6-787B-4A28-BF0D-1980346A2B87}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11190" xr2:uid="{4A0416FB-2C84-4E89-A2FF-929A6C4E2758}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11196"/>
   </bookViews>
   <sheets>
     <sheet name="Tube" sheetId="1" r:id="rId1"/>
     <sheet name="디스크립션" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="166">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -390,22 +389,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jake_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_enhancer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_cooler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제이크 스타일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>107식 스타일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -430,14 +413,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>제이크 인핸서</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제이크 쿨러</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{(0.7)}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -474,10 +449,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{(jake_attack, 4, 4)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>no107_skill</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -486,10 +457,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jake_attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -511,13 +478,217 @@
   </si>
   <si>
     <t>relic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_B_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_B_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_B_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_R_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_R_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_R_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크B 스타일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크B 인핸서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크B 쿨러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크R 스타일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크R 인핸서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이크R 쿨러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_B_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_R_attack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(0.3)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(jake_B_attack, 4, 4)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(jake_R_skill, 0,5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나01 스타일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나01 인핸서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나01 쿨러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나02 스타일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나02 인핸서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나02 쿨러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나02 렐릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gangster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1.0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina01_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina01_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina01_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina02_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina02_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina02_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina02_relic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina_skill00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina_skill01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(doncinal, 1, 5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>melee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(doncinal, 0, 1)}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,20 +1072,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C425640-F0D4-4DE1-87FB-B938FDD96FB7}">
-  <dimension ref="A1:Q23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +1144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1100</v>
       </c>
@@ -996,7 +1173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1101</v>
       </c>
@@ -1025,7 +1202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1102</v>
       </c>
@@ -1054,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2100</v>
       </c>
@@ -1074,7 +1251,7 @@
         <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M5" t="s">
         <v>28</v>
@@ -1086,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2101</v>
       </c>
@@ -1118,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2102</v>
       </c>
@@ -1150,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>2103</v>
       </c>
@@ -1182,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2104</v>
       </c>
@@ -1214,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>3100</v>
       </c>
@@ -1237,7 +1414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>3101</v>
       </c>
@@ -1260,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>3102</v>
       </c>
@@ -1283,53 +1460,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>4100</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="Q13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>4101</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="Q14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>5100</v>
       </c>
@@ -1337,7 +1514,7 @@
         <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1346,22 +1523,22 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>5101</v>
       </c>
@@ -1369,7 +1546,7 @@
         <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -1378,16 +1555,16 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K16" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>5102</v>
       </c>
@@ -1395,7 +1572,7 @@
         <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -1404,13 +1581,13 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="P17">
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>5103</v>
       </c>
@@ -1418,7 +1595,7 @@
         <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1427,22 +1604,22 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H18" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>5104</v>
       </c>
@@ -1450,7 +1627,7 @@
         <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1459,16 +1636,16 @@
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>5105</v>
       </c>
@@ -1476,7 +1653,7 @@
         <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1485,21 +1662,21 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="P20">
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>5106</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -1508,30 +1685,30 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="H21" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="J21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>5107</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -1540,24 +1717,24 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>5108</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -1566,10 +1743,276 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="P23">
         <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>5109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+      <c r="L24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>5110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>5111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>129</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>5112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" t="s">
+        <v>164</v>
+      </c>
+      <c r="J27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>5113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K28" t="s">
+        <v>165</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>5114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" t="s">
+        <v>148</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>5115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" t="s">
+        <v>162</v>
+      </c>
+      <c r="H30" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" t="s">
+        <v>153</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>5116</v>
+      </c>
+      <c r="B31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L31" t="s">
+        <v>163</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>5117</v>
+      </c>
+      <c r="B32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>149</v>
+      </c>
+      <c r="P32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>5118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1580,21 +2023,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A04AEDB-2076-4335-A064-676E089814A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>53</v>
       </c>
@@ -1608,7 +2051,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>49</v>
       </c>
@@ -1619,7 +2062,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>50</v>
       </c>
@@ -1630,7 +2073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -1641,7 +2084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -1652,7 +2095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>56</v>
       </c>
@@ -1663,7 +2106,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -1674,7 +2117,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -1685,7 +2128,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -1699,7 +2142,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -1710,7 +2153,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>61</v>
       </c>
@@ -1721,7 +2164,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>62</v>
       </c>
@@ -1732,7 +2175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>63</v>
       </c>
@@ -1743,7 +2186,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>64</v>
       </c>
@@ -1754,7 +2197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>65</v>
       </c>
@@ -1765,7 +2208,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>66</v>
       </c>
@@ -1776,7 +2219,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>67</v>
       </c>
@@ -1787,7 +2230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>85</v>
       </c>

</xml_diff>